<commit_message>
track user location performance ok
</commit_message>
<xml_diff>
--- a/TourGuide+Performance+Graphs.xlsx
+++ b/TourGuide+Performance+Graphs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -310,6 +310,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -417,6 +418,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -493,11 +495,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="59443340"/>
-        <c:axId val="19239268"/>
+        <c:axId val="93397537"/>
+        <c:axId val="22881133"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59443340"/>
+        <c:axId val="93397537"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +528,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19239268"/>
+        <c:crossAx val="22881133"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -534,7 +536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19239268"/>
+        <c:axId val="22881133"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +608,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59443340"/>
+        <c:crossAx val="93397537"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -739,6 +741,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -834,6 +837,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -877,10 +881,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -898,11 +902,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="41559767"/>
-        <c:axId val="16491865"/>
+        <c:axId val="94341612"/>
+        <c:axId val="74572371"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41559767"/>
+        <c:axId val="94341612"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +935,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16491865"/>
+        <c:crossAx val="74572371"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -939,7 +943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16491865"/>
+        <c:axId val="74572371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,7 +1015,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41559767"/>
+        <c:crossAx val="94341612"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1072,9 +1076,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>807480</xdr:colOff>
+      <xdr:colOff>807120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1082,8 +1086,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4001760" y="200160"/>
-        <a:ext cx="5714640" cy="3533400"/>
+        <a:off x="4006800" y="200160"/>
+        <a:ext cx="5722200" cy="3533040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1107,9 +1111,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>817200</xdr:colOff>
+      <xdr:colOff>816840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1117,8 +1121,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4011480" y="190440"/>
-        <a:ext cx="5714640" cy="3533400"/>
+        <a:off x="4016520" y="190440"/>
+        <a:ext cx="5722200" cy="3533040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1138,11 +1142,11 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1247,11 +1251,11 @@
   </sheetPr>
   <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
@@ -1286,7 +1290,7 @@
         <v>472</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,7 +1301,7 @@
         <v>5820</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
calculateRewards update and test ok
</commit_message>
<xml_diff>
--- a/TourGuide+Performance+Graphs.xlsx
+++ b/TourGuide+Performance+Graphs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t xml:space="preserve">Users</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t xml:space="preserve">Get Rewards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unt</t>
   </si>
 </sst>
 </file>
@@ -495,11 +498,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="93397537"/>
-        <c:axId val="22881133"/>
+        <c:axId val="32405627"/>
+        <c:axId val="80580310"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93397537"/>
+        <c:axId val="32405627"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +531,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22881133"/>
+        <c:crossAx val="80580310"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -536,7 +539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22881133"/>
+        <c:axId val="80580310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -608,7 +611,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93397537"/>
+        <c:crossAx val="32405627"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -878,16 +881,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>249</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>26000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -902,11 +905,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="94341612"/>
-        <c:axId val="74572371"/>
+        <c:axId val="22046293"/>
+        <c:axId val="29637029"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94341612"/>
+        <c:axId val="22046293"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -935,7 +938,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74572371"/>
+        <c:crossAx val="29637029"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -943,7 +946,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74572371"/>
+        <c:axId val="29637029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1015,7 +1018,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94341612"/>
+        <c:crossAx val="22046293"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1076,9 +1079,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>807120</xdr:colOff>
+      <xdr:colOff>806400</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1086,8 +1089,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4006800" y="200160"/>
-        <a:ext cx="5722200" cy="3533040"/>
+        <a:off x="4016880" y="200160"/>
+        <a:ext cx="5736600" cy="3532320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1111,9 +1114,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>816840</xdr:colOff>
+      <xdr:colOff>816120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1121,8 +1124,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4016520" y="190440"/>
-        <a:ext cx="5722200" cy="3533040"/>
+        <a:off x="4370760" y="190440"/>
+        <a:ext cx="5736600" cy="3532320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1140,13 +1143,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1177,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="n">
         <v>1000</v>
       </c>
@@ -1230,6 +1233,11 @@
       </c>
       <c r="D8" s="1" t="n">
         <v>374</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="0" t="n">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -1249,13 +1257,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D6"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.56"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
@@ -1279,7 +1290,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,7 +1301,7 @@
         <v>472</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,7 +1312,7 @@
         <v>5820</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>249</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,7 +1323,15 @@
         <v>64020</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0</v>
+        <v>26000</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>